<commit_message>
Prova Testes de Software
</commit_message>
<xml_diff>
--- a/selenium-lab-thalles-nascimento/selenium-lab-main/Planilha_de_planejamento_de_testes.xlsx
+++ b/selenium-lab-thalles-nascimento/selenium-lab-main/Planilha_de_planejamento_de_testes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Prova Testes de Software\selenium-lab-thalles-nascimento\selenium-lab-main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A398C7D-EF6E-4A15-9F13-A2603161245A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77E405C9-45EC-4287-8884-D10DE7272F94}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -121,7 +121,7 @@
     <t>Deve negar produtos iguais</t>
   </si>
   <si>
-    <t>Aceitar letras nos campos de números e números no campo de números</t>
+    <t>Não aceitar letras nos campos de números e números no campo de números</t>
   </si>
 </sst>
 </file>
@@ -3747,7 +3747,7 @@
   <dimension ref="B1:D1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3876,7 +3876,7 @@
         <v>31</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="2:4" ht="28.5" x14ac:dyDescent="0.2">

</xml_diff>